<commit_message>
Updated values based on 2.1
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemantsatam/projects/upGrad/AI_ML/Investment Analysis Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemantsatam/projects/GitHub/AI_ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DAE52D74-CF87-B049-BAFF-13131521E28A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{354213EB-3784-E143-AEE9-B0B8F69AC494}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26140" yWindow="4820" windowWidth="24660" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2020" yWindow="3460" windowWidth="24660" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -366,10 +366,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>permalink = 66368
-company_permalink=114949</t>
-  </si>
-  <si>
     <t>Venture</t>
   </si>
   <si>
@@ -380,6 +376,10 @@
   </si>
   <si>
     <t>Mauritius (MUR)</t>
+  </si>
+  <si>
+    <t>1. Values of key columns have different case
+2. Null values exists in raised_amount_usd column</t>
   </si>
 </sst>
 </file>
@@ -664,6 +664,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -695,12 +701,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1031,23 +1031,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1068,7 +1068,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="17">
-        <v>90247</v>
+        <v>66368</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1079,7 +1079,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="17">
-        <v>66368</v>
+        <v>66370</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1112,7 +1112,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1156,21 +1156,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1190,8 +1190,8 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="36">
-        <v>11748949</v>
+      <c r="C5" s="25">
+        <v>10634054</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1201,8 +1201,8 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="36">
-        <v>958694</v>
+      <c r="C6" s="25">
+        <v>764564</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1212,8 +1212,8 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="36">
-        <v>719818</v>
+      <c r="C7" s="25">
+        <v>556607</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1223,8 +1223,8 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="36">
-        <v>73308593</v>
+      <c r="C8" s="25">
+        <v>62111788</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1234,8 +1234,8 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>43</v>
+      <c r="C9" s="25" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1262,7 +1262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1274,21 +1274,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -1308,8 +1308,8 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>44</v>
+      <c r="C5" s="26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1319,8 +1319,8 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>45</v>
+      <c r="C6" s="26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1330,8 +1330,8 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>46</v>
+      <c r="C7" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1371,23 +1371,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">

</xml_diff>

<commit_message>
solution for table 3.1 added
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemantsatam/projects/GitHub/AI_ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{354213EB-3784-E143-AEE9-B0B8F69AC494}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{618B051F-E411-5148-B280-FFBA7B1430F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2020" yWindow="3460" windowWidth="24660" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,17 +369,17 @@
     <t>Venture</t>
   </si>
   <si>
-    <t>Grenada (GRD)</t>
-  </si>
-  <si>
-    <t>Bermuda (BMU)</t>
-  </si>
-  <si>
-    <t>Mauritius (MUR)</t>
-  </si>
-  <si>
     <t>1. Values of key columns have different case
 2. Null values exists in raised_amount_usd column</t>
+  </si>
+  <si>
+    <t>United States (USA)</t>
+  </si>
+  <si>
+    <t>United Kingdom (GBR)</t>
+  </si>
+  <si>
+    <t>India (IND)</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1112,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1320,7 +1320,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1331,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated XL and ppt
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hemantsatam/projects/GitHub/AI_ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{618B051F-E411-5148-B280-FFBA7B1430F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C3B52D8E-4D67-A74D-ADDD-BF9F0CE078F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="3460" windowWidth="24660" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18320" yWindow="6920" windowWidth="32580" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>C1</t>
   </si>
@@ -369,10 +369,6 @@
     <t>Venture</t>
   </si>
   <si>
-    <t>1. Values of key columns have different case
-2. Null values exists in raised_amount_usd column</t>
-  </si>
-  <si>
     <t>United States (USA)</t>
   </si>
   <si>
@@ -380,6 +376,36 @@
   </si>
   <si>
     <t>India (IND)</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Cleantech / Semiconductors</t>
+  </si>
+  <si>
+    <t>Social, Finance, Analytics, Advertising Count</t>
+  </si>
+  <si>
+    <t>/organization/social-finance</t>
+  </si>
+  <si>
+    <t>/organization/freescale</t>
+  </si>
+  <si>
+    <t>/organization/oneweb</t>
+  </si>
+  <si>
+    <t>/organization/immunocore</t>
+  </si>
+  <si>
+    <t>News, Search and Messaging</t>
+  </si>
+  <si>
+    <t>/organization/flipkart</t>
+  </si>
+  <si>
+    <t>/organization/quikr-india</t>
   </si>
 </sst>
 </file>
@@ -596,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -670,6 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1019,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1031,23 +1058,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1111,8 +1138,8 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>43</v>
+      <c r="C9" s="16">
+        <v>114942</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1144,7 +1171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1156,21 +1183,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -1262,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1274,21 +1301,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -1309,7 +1336,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1320,7 +1347,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1331,7 +1358,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1357,37 +1384,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="56.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="3" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
@@ -1413,9 +1438,15 @@
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="17">
+        <v>37248</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2207</v>
+      </c>
+      <c r="E5" s="17">
+        <v>927</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
@@ -1424,9 +1455,15 @@
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="27">
+        <v>422510842796</v>
+      </c>
+      <c r="D6" s="17">
+        <v>20245627416</v>
+      </c>
+      <c r="E6" s="17">
+        <v>14391858718</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
@@ -1435,9 +1472,15 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
@@ -1446,9 +1489,15 @@
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
@@ -1457,9 +1506,15 @@
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
@@ -1468,9 +1523,15 @@
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="17">
+        <v>8693</v>
+      </c>
+      <c r="D10" s="17">
+        <v>571</v>
+      </c>
+      <c r="E10" s="17">
+        <v>329</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
@@ -1479,9 +1540,15 @@
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="17">
+        <v>8113</v>
+      </c>
+      <c r="D11" s="17">
+        <v>456</v>
+      </c>
+      <c r="E11" s="17">
+        <v>154</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
@@ -1490,9 +1557,15 @@
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="17">
+        <v>7042</v>
+      </c>
+      <c r="D12" s="17">
+        <v>408</v>
+      </c>
+      <c r="E12" s="17">
+        <v>133</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
@@ -1501,9 +1574,15 @@
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
@@ -1512,9 +1591,15 @@
       <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1522,7 +1607,7 @@
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="B5">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1530,7 +1615,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1541,8 +1626,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E14">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="A5:E7 A8:D8 A9:E14">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1554,7 +1639,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A14">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1563,6 +1648,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>